<commit_message>
alpha input, copy code to vanish TR
</commit_message>
<xml_diff>
--- a/PCB/TeensyROM pin-reg map.xlsx
+++ b/PCB/TeensyROM pin-reg map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB49F13-025E-49D4-9939-DE306684F5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBC3A5F-80AD-48EE-8CA2-0BB8B1E35B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="-15435" windowWidth="17250" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Map" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="223">
   <si>
     <t>Teensy 4.0</t>
   </si>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>Reset Out</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
+  <si>
+    <t>Flash/SRAM locations</t>
   </si>
 </sst>
 </file>
@@ -724,7 +730,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -770,6 +776,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -891,6 +903,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1317,7 +1330,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2325,9 +2338,15 @@
       <c r="I27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>205</v>
+      </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
@@ -2356,9 +2375,15 @@
       <c r="I28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L28" s="22" t="s">
+        <v>205</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
@@ -2549,9 +2574,15 @@
       <c r="I33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" s="22" t="s">
+        <v>205</v>
+      </c>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
@@ -2580,8 +2611,15 @@
       <c r="I34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L34" s="22" t="s">
+        <v>205</v>
+      </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
@@ -2964,7 +3002,7 @@
       <c r="G45" s="1">
         <v>15</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="23">
         <v>42</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -2974,7 +3012,9 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
+      <c r="N45" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
@@ -2987,7 +3027,7 @@
       <c r="G46" s="1">
         <v>14</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="23">
         <v>43</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -2997,7 +3037,9 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
+      <c r="N46" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
@@ -3010,7 +3052,7 @@
       <c r="G47" s="1">
         <v>13</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="23">
         <v>44</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3020,7 +3062,9 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
+      <c r="N47" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
@@ -3033,7 +3077,7 @@
       <c r="G48" s="1">
         <v>12</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="23">
         <v>45</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -3043,7 +3087,9 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
+      <c r="N48" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
@@ -3056,7 +3102,7 @@
       <c r="G49" s="1">
         <v>17</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="23">
         <v>46</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -3066,7 +3112,9 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="N49" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
@@ -3079,7 +3127,7 @@
       <c r="G50" s="1">
         <v>16</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="23">
         <v>47</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -3089,7 +3137,9 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
+      <c r="N50" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
@@ -3108,17 +3158,13 @@
       <c r="I51" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L51" s="22" t="s">
-        <v>205</v>
-      </c>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
+      <c r="N51" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
@@ -3137,17 +3183,13 @@
       <c r="I52" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L52" s="22" t="s">
-        <v>205</v>
-      </c>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+      <c r="N52" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
@@ -3170,7 +3212,9 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
+      <c r="N53" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
@@ -3193,7 +3237,9 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
+      <c r="N54" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
@@ -3212,17 +3258,13 @@
       <c r="I55" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L55" s="22" t="s">
-        <v>205</v>
-      </c>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
       <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
+      <c r="N55" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
@@ -3241,17 +3283,13 @@
       <c r="I56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L56" s="22" t="s">
-        <v>205</v>
-      </c>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
+      <c r="N56" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
@@ -3274,7 +3312,9 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
+      <c r="N57" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:N57" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">

</xml_diff>

<commit_message>
Reset in changed to Reset button only
</commit_message>
<xml_diff>
--- a/PCB/TeensyROM pin-reg map.xlsx
+++ b/PCB/TeensyROM pin-reg map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A750BCF7-041E-436C-87B8-BAD6AF548223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21EE2B4-9576-4F36-83C3-9196B397BAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1332" yWindow="4608" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Map" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Exp Port" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin Map'!$B$2:$P$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin Map'!$B$2:$O$59</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="279">
   <si>
     <t>Teensy 4.0</t>
   </si>
@@ -655,9 +655,6 @@
     <t>MM Grey</t>
   </si>
   <si>
-    <t>Not Connected/unused</t>
-  </si>
-  <si>
     <t>G3 Blu</t>
   </si>
   <si>
@@ -743,29 +740,6 @@
   </si>
   <si>
     <t>Direction (T4 pov)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>out only</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to OC buff</t>
-    </r>
   </si>
   <si>
     <r>
@@ -791,18 +765,9 @@
     </r>
   </si>
   <si>
-    <t>bi-dir</t>
-  </si>
-  <si>
     <t>Mostly (all?) input, use OC buff for inp??</t>
   </si>
   <si>
-    <t>OC-out</t>
-  </si>
-  <si>
-    <t>OC-in</t>
-  </si>
-  <si>
     <t>In(no out?)</t>
   </si>
   <si>
@@ -839,9 +804,6 @@
     <t>315-PA0035C-ND  PA0035C   Chip Quik Inc.   TSSOP-20 TO DIP-20 SMT ADAPTER (</t>
   </si>
   <si>
-    <t>to/from Bi-Dir buffer FET</t>
-  </si>
-  <si>
     <t>BSH105,215   MOSFET N-CH 20V 1.05A TO236AB</t>
   </si>
   <si>
@@ -927,6 +889,35 @@
   </si>
   <si>
     <t>Reset out</t>
+  </si>
+  <si>
+    <t>Change to/from Bi-Dir buffer FET???</t>
+  </si>
+  <si>
+    <t>From button</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OC buffer</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1120,7 +1111,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1152,12 +1143,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1186,31 +1173,15 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{90DC91C5-8A25-4FD1-9045-E2CBF1985420}"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1282,6 +1253,14 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1694,11 +1673,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:P59"/>
+  <dimension ref="B1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1709,11 +1688,10 @@
     <col min="11" max="11" width="8.33203125" style="20" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1"/>
-    <col min="16" max="16" width="49.44140625" customWidth="1"/>
+    <col min="15" max="15" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
+    <row r="1" spans="2:15">
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1734,9 +1712,8 @@
       <c r="M1" s="10"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="2:16" s="25" customFormat="1" ht="28.8">
+    </row>
+    <row r="2" spans="2:15" s="23" customFormat="1" ht="28.8">
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1749,865 +1726,834 @@
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="L2" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="M2" s="30" t="s">
+      <c r="K2" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="M2" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31" t="s">
+      <c r="O2" s="29" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:16">
-      <c r="B3" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="37">
-        <v>10</v>
-      </c>
-      <c r="D3" s="37">
-        <v>6</v>
-      </c>
-      <c r="E3" s="37"/>
+    <row r="3" spans="2:15">
+      <c r="B3" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="35">
+        <v>3</v>
+      </c>
+      <c r="D3" s="35">
+        <v>0</v>
+      </c>
+      <c r="E3" s="35"/>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="1">
-        <v>10</v>
-      </c>
-      <c r="H3" s="16">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>252</v>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="O3" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="P3" s="40"/>
-    </row>
-    <row r="4" spans="2:16">
-      <c r="B4" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="37">
-        <v>11</v>
-      </c>
-      <c r="D4" s="37">
-        <v>9</v>
-      </c>
-      <c r="E4" s="37"/>
+        <v>55</v>
+      </c>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="B4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="35">
+        <v>2</v>
+      </c>
+      <c r="D4" s="35">
+        <v>1</v>
+      </c>
+      <c r="E4" s="35"/>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1">
-        <v>11</v>
-      </c>
-      <c r="H4" s="16">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="22">
-        <v>9</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="O4" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="2:16">
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1">
-        <v>13</v>
-      </c>
-      <c r="H5" s="16">
-        <v>25</v>
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>127</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="K5" s="19"/>
       <c r="L5" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>204</v>
+        <v>40</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16">
+        <v>55</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:15">
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3">
-        <v>30</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1">
-        <v>23</v>
-      </c>
-      <c r="H6" s="16">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K6" s="22">
-        <v>13</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="K6" s="19"/>
       <c r="L6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>204</v>
+        <v>40</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16">
+        <v>196</v>
+      </c>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="2:15">
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G7" s="1">
-        <v>22</v>
-      </c>
-      <c r="H7" s="16">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>280</v>
+      <c r="J7" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="K7" s="19"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="2:16">
+    </row>
+    <row r="8" spans="2:15">
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1">
-        <v>12</v>
-      </c>
-      <c r="H8" s="16">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="22">
-        <v>8</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="P8" s="21"/>
-    </row>
-    <row r="9" spans="2:16">
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>223</v>
+      <c r="J8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="37">
+        <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>61</v>
+      <c r="J9" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O9" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="9">
+        <v>17</v>
+      </c>
+      <c r="H10" s="1">
+        <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="L10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-    </row>
-    <row r="11" spans="2:16">
+      <c r="J10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="2:15">
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3</v>
+        <v>37</v>
+      </c>
+      <c r="G11" s="9">
+        <v>16</v>
       </c>
       <c r="H11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>32</v>
+      <c r="J11" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="K11" s="19"/>
       <c r="L11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="2:16">
+    </row>
+    <row r="12" spans="2:15">
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1">
-        <v>2</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="H12" s="37">
+        <v>9</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="K12" s="19">
+        <v>9</v>
+      </c>
       <c r="L12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
       <c r="O12" s="1"/>
-      <c r="P12" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16">
+    </row>
+    <row r="13" spans="2:15">
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="1">
-        <v>4</v>
+        <v>37</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="22"/>
+      <c r="J13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="19"/>
       <c r="L13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="2:16">
+    </row>
+    <row r="14" spans="2:15">
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="1">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="G14" s="9">
+        <v>2</v>
       </c>
       <c r="H14" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="22"/>
+      <c r="J14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="19"/>
       <c r="L14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>196</v>
+        <v>55</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="2:16">
+    </row>
+    <row r="15" spans="2:15">
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="1">
-        <v>6</v>
+        <v>37</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="22"/>
+      <c r="J15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="19"/>
       <c r="L15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>205</v>
+        <v>55</v>
       </c>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="2:16">
+    </row>
+    <row r="16" spans="2:15">
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="1">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="G16" s="9">
+        <v>3</v>
       </c>
       <c r="H16" s="1">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="22"/>
+      <c r="J16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="19"/>
       <c r="L16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="2:16">
+        <v>55</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="9">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="G17" s="2">
+        <v>18</v>
       </c>
       <c r="H17" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="22"/>
+      <c r="J17" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K17" s="19"/>
       <c r="L17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="2:16">
+    </row>
+    <row r="18" spans="2:15">
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="9">
-        <v>16</v>
+        <v>36</v>
+      </c>
+      <c r="G18" s="2">
+        <v>19</v>
       </c>
       <c r="H18" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="22"/>
+      <c r="J18" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K18" s="19"/>
       <c r="L18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="2:16">
+    </row>
+    <row r="19" spans="2:15">
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G19" s="2">
+        <v>23</v>
       </c>
       <c r="H19" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="22"/>
+      <c r="J19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="K19" s="19"/>
       <c r="L19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="2:16">
+    </row>
+    <row r="20" spans="2:15">
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="9">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="G20" s="2">
+        <v>22</v>
       </c>
       <c r="H20" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" s="22"/>
+      <c r="J20" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="K20" s="19"/>
       <c r="L20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="2:16">
+    </row>
+    <row r="21" spans="2:15">
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="9">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="G21" s="2">
+        <v>17</v>
       </c>
       <c r="H21" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="22"/>
+      <c r="J21" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="K21" s="19"/>
       <c r="L21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-    </row>
-    <row r="22" spans="2:16">
+    </row>
+    <row r="22" spans="2:15">
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="9">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="G22" s="2">
+        <v>16</v>
       </c>
       <c r="H22" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="22"/>
+      <c r="J22" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K22" s="19"/>
       <c r="L22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16">
+    </row>
+    <row r="23" spans="2:15">
       <c r="B23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D23" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G23" s="2">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H23" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="K23" s="22"/>
+        <v>25</v>
+      </c>
+      <c r="K23" s="19"/>
       <c r="L23" s="1" t="s">
         <v>40</v>
       </c>
@@ -2615,38 +2561,37 @@
         <v>51</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-    </row>
-    <row r="24" spans="2:16">
+    </row>
+    <row r="24" spans="2:15">
       <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="1">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D24" s="1">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G24" s="2">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H24" s="1">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="K24" s="22"/>
+        <v>26</v>
+      </c>
+      <c r="K24" s="19"/>
       <c r="L24" s="1" t="s">
         <v>40</v>
       </c>
@@ -2654,30 +2599,29 @@
         <v>51</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="2:16">
+    </row>
+    <row r="25" spans="2:15">
       <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D25" s="1">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G25" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H25" s="1">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>43</v>
@@ -2685,7 +2629,7 @@
       <c r="J25" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="K25" s="22"/>
+      <c r="K25" s="19"/>
       <c r="L25" s="1" t="s">
         <v>40</v>
       </c>
@@ -2693,38 +2637,37 @@
         <v>51</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>55</v>
+        <v>190</v>
       </c>
       <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="2:16">
+    </row>
+    <row r="26" spans="2:15">
       <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D26" s="1">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G26" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H26" s="1">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="K26" s="22"/>
+        <v>216</v>
+      </c>
+      <c r="K26" s="19"/>
       <c r="L26" s="1" t="s">
         <v>40</v>
       </c>
@@ -2732,116 +2675,127 @@
         <v>51</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>55</v>
+        <v>203</v>
       </c>
       <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="2:16">
+    </row>
+    <row r="27" spans="2:15">
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="1">
-        <v>17</v>
-      </c>
-      <c r="D27" s="1">
-        <v>18</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="D27" s="3">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="2">
-        <v>17</v>
+      <c r="G27" s="1">
+        <v>12</v>
       </c>
       <c r="H27" s="1">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="K27" s="22"/>
+      <c r="J27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" s="19">
+        <v>4</v>
+      </c>
       <c r="L27" s="1" t="s">
-        <v>40</v>
+        <v>235</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>51</v>
+        <v>278</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-    </row>
-    <row r="28" spans="2:16">
+        <v>226</v>
+      </c>
+      <c r="O27" s="17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15">
       <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="1">
-        <v>16</v>
-      </c>
-      <c r="D28" s="1">
-        <v>19</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D28" s="3">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="2">
-        <v>16</v>
-      </c>
-      <c r="H28" s="1">
-        <v>19</v>
+      <c r="G28" s="1">
+        <v>13</v>
+      </c>
+      <c r="H28" s="37">
+        <v>25</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="K28" s="22"/>
+      <c r="J28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="L28" s="1" t="s">
-        <v>40</v>
+        <v>238</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="2:16">
+        <v>229</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15">
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="1">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3">
         <v>26</v>
       </c>
-      <c r="D29" s="1">
-        <v>20</v>
-      </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G29" s="2">
+        <v>30</v>
+      </c>
+      <c r="H29" s="1">
         <v>26</v>
-      </c>
-      <c r="H29" s="1">
-        <v>20</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K29" s="22"/>
+        <v>140</v>
+      </c>
+      <c r="K29" s="19"/>
       <c r="L29" s="1" t="s">
         <v>40</v>
       </c>
@@ -2849,38 +2803,39 @@
         <v>51</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-    </row>
-    <row r="30" spans="2:16">
+    </row>
+    <row r="30" spans="2:15">
       <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="1">
+        <v>31</v>
+      </c>
+      <c r="D30" s="3">
         <v>27</v>
       </c>
-      <c r="D30" s="1">
-        <v>21</v>
-      </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G30" s="2">
+        <v>31</v>
+      </c>
+      <c r="H30" s="1">
         <v>27</v>
-      </c>
-      <c r="H30" s="1">
-        <v>21</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K30" s="22"/>
+        <v>136</v>
+      </c>
+      <c r="K30" s="19"/>
       <c r="L30" s="1" t="s">
         <v>40</v>
       </c>
@@ -2888,38 +2843,41 @@
         <v>51</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-    </row>
-    <row r="31" spans="2:16">
+    </row>
+    <row r="31" spans="2:15">
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1">
-        <v>24</v>
-      </c>
-      <c r="D31" s="1">
-        <v>22</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="D31" s="3">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G31" s="2">
-        <v>24</v>
-      </c>
-      <c r="H31" s="1">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="G31" s="1">
+        <v>18</v>
+      </c>
+      <c r="H31" s="37">
+        <v>28</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="K31" s="22"/>
+      <c r="J31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K31" s="19">
+        <v>6</v>
+      </c>
       <c r="L31" s="1" t="s">
         <v>40</v>
       </c>
@@ -2927,38 +2885,41 @@
         <v>51</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-    </row>
-    <row r="32" spans="2:16">
+        <v>225</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15">
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1">
-        <v>23</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D32" s="3">
+        <v>29</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" s="2">
-        <v>25</v>
+        <v>39</v>
+      </c>
+      <c r="G32" s="1">
+        <v>31</v>
       </c>
       <c r="H32" s="1">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="K32" s="22"/>
+      <c r="J32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K32" s="19"/>
       <c r="L32" s="1" t="s">
         <v>40</v>
       </c>
@@ -2966,270 +2927,247 @@
         <v>51</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-    </row>
-    <row r="33" spans="2:16">
+    </row>
+    <row r="33" spans="2:15">
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D33" s="3">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G33" s="1">
-        <v>12</v>
-      </c>
-      <c r="H33" s="1">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="H33" s="37">
+        <v>30</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K33" s="22">
-        <v>4</v>
+        <v>93</v>
+      </c>
+      <c r="K33" s="19">
+        <v>13</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M33" s="16" t="s">
-        <v>204</v>
+        <v>42</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="P33" s="16" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16">
+        <v>224</v>
+      </c>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="2:15">
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D34" s="3">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="2">
-        <v>30</v>
-      </c>
-      <c r="H34" s="1">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="G34" s="1">
+        <v>22</v>
+      </c>
+      <c r="H34" s="37">
+        <v>31</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K34" s="22"/>
-      <c r="L34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="2:16">
+      <c r="J34" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="K34" s="19"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
       <c r="B35" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D35" s="3">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="2">
-        <v>31</v>
-      </c>
-      <c r="H35" s="1">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="G35" s="1">
+        <v>12</v>
+      </c>
+      <c r="H35" s="37">
+        <v>32</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="K35" s="22"/>
+      <c r="J35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" s="19">
+        <v>8</v>
+      </c>
       <c r="L35" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="2:16">
+    </row>
+    <row r="36" spans="2:15">
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D36" s="3">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G36" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="H36" s="1">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K36" s="22">
-        <v>6</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M36" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>226</v>
-      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-      <c r="P36" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16">
+    </row>
+    <row r="37" spans="2:15">
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D37" s="3">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G37" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H37" s="1">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K37" s="22"/>
-      <c r="L37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>197</v>
-      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-    </row>
-    <row r="38" spans="2:16">
+    </row>
+    <row r="38" spans="2:15">
       <c r="B38" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D38" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G38" s="1">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="H38" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="1"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="N38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K38" s="19"/>
+      <c r="L38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-    </row>
-    <row r="39" spans="2:16">
+    </row>
+    <row r="39" spans="2:15">
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D39" s="3">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>28</v>
@@ -3237,34 +3175,39 @@
       <c r="F39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="1">
-        <v>29</v>
+      <c r="G39" s="9">
+        <v>18</v>
       </c>
       <c r="H39" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J39" s="1"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="N39" s="1"/>
+      <c r="J39" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" s="19"/>
+      <c r="L39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-    </row>
-    <row r="40" spans="2:16">
+    </row>
+    <row r="40" spans="2:15">
       <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D40" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>28</v>
@@ -3272,142 +3215,131 @@
       <c r="F40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G40" s="1">
-        <v>28</v>
+      <c r="G40" s="9">
+        <v>19</v>
       </c>
       <c r="H40" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K40" s="22"/>
+      <c r="J40" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="19"/>
       <c r="L40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="2:16">
+    </row>
+    <row r="41" spans="2:15">
       <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D41" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G41" s="9">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="G41" s="2">
+        <v>28</v>
       </c>
       <c r="H41" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" s="22"/>
+      <c r="J41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41" s="19"/>
       <c r="L41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>55</v>
+        <v>193</v>
       </c>
       <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-    </row>
-    <row r="42" spans="2:16">
+    </row>
+    <row r="42" spans="2:15">
       <c r="B42" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C42" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D42" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G42" s="9">
-        <v>19</v>
+        <v>36</v>
+      </c>
+      <c r="G42" s="2">
+        <v>29</v>
       </c>
       <c r="H42" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J42" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K42" s="22"/>
+      <c r="J42" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K42" s="19"/>
       <c r="L42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>55</v>
+        <v>194</v>
       </c>
       <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-    </row>
-    <row r="43" spans="2:16">
-      <c r="B43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="1">
-        <v>17</v>
-      </c>
-      <c r="D43" s="3">
-        <v>38</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>28</v>
-      </c>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G43" s="2">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H43" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K43" s="22"/>
+        <v>211</v>
+      </c>
+      <c r="K43" s="19"/>
       <c r="L43" s="1" t="s">
         <v>40</v>
       </c>
@@ -3415,40 +3347,31 @@
         <v>51</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>193</v>
+        <v>55</v>
       </c>
       <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-    </row>
-    <row r="44" spans="2:16">
-      <c r="B44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="1">
-        <v>16</v>
-      </c>
-      <c r="D44" s="3">
-        <v>39</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>28</v>
-      </c>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G44" s="2">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H44" s="1">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="K44" s="22"/>
+        <v>212</v>
+      </c>
+      <c r="K44" s="19"/>
       <c r="L44" s="1" t="s">
         <v>40</v>
       </c>
@@ -3456,78 +3379,63 @@
         <v>51</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>194</v>
+        <v>55</v>
       </c>
       <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-    </row>
-    <row r="45" spans="2:16">
+    </row>
+    <row r="45" spans="2:15">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G45" s="2">
-        <v>20</v>
-      </c>
-      <c r="H45" s="1">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="G45" s="1">
+        <v>15</v>
+      </c>
+      <c r="H45" s="17">
+        <v>42</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="K45" s="22"/>
-      <c r="L45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-    </row>
-    <row r="46" spans="2:16">
+        <v>28</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G46" s="2">
-        <v>21</v>
-      </c>
-      <c r="H46" s="1">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="G46" s="1">
+        <v>14</v>
+      </c>
+      <c r="H46" s="17">
+        <v>43</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="K46" s="22"/>
-      <c r="L46" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-    </row>
-    <row r="47" spans="2:16">
+        <v>28</v>
+      </c>
+      <c r="J46" s="1"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3536,25 +3444,24 @@
         <v>38</v>
       </c>
       <c r="G47" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H47" s="17">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J47" s="1"/>
-      <c r="K47" s="22"/>
+      <c r="K47" s="19"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="48" spans="2:16">
+      <c r="O47" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -3563,25 +3470,24 @@
         <v>38</v>
       </c>
       <c r="G48" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H48" s="17">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J48" s="1"/>
-      <c r="K48" s="22"/>
+      <c r="K48" s="19"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16">
+      <c r="O48" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -3590,25 +3496,24 @@
         <v>38</v>
       </c>
       <c r="G49" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H49" s="17">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J49" s="1"/>
-      <c r="K49" s="22"/>
+      <c r="K49" s="19"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16">
+      <c r="O49" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -3617,10 +3522,10 @@
         <v>38</v>
       </c>
       <c r="G50" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H50" s="17">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>28</v>
@@ -3630,24 +3535,23 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16">
+      <c r="O50" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G51" s="1">
-        <v>17</v>
-      </c>
-      <c r="H51" s="17">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="H51" s="3">
+        <v>48</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>28</v>
@@ -3657,24 +3561,23 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:15">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G52" s="1">
-        <v>16</v>
-      </c>
-      <c r="H52" s="17">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="H52" s="3">
+        <v>49</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>28</v>
@@ -3684,12 +3587,11 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:15">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3698,10 +3600,10 @@
         <v>39</v>
       </c>
       <c r="G53" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H53" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>28</v>
@@ -3711,12 +3613,11 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16">
+      <c r="O53" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -3725,10 +3626,10 @@
         <v>39</v>
       </c>
       <c r="G54" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H54" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>28</v>
@@ -3738,12 +3639,11 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16">
+      <c r="O54" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -3752,10 +3652,10 @@
         <v>39</v>
       </c>
       <c r="G55" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H55" s="3">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>28</v>
@@ -3765,12 +3665,11 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16">
+      <c r="O55" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -3779,10 +3678,10 @@
         <v>39</v>
       </c>
       <c r="G56" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H56" s="3">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>28</v>
@@ -3792,12 +3691,11 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="57" spans="2:16">
+      <c r="O56" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -3806,10 +3704,10 @@
         <v>39</v>
       </c>
       <c r="G57" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H57" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>28</v>
@@ -3819,69 +3717,80 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="58" spans="2:16">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="O57" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
       <c r="F58" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G58" s="1">
-        <v>25</v>
-      </c>
-      <c r="H58" s="3">
-        <v>53</v>
+        <v>223</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J58" s="1"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="J58" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="K58" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
+      <c r="N58" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="O58" s="1"/>
-      <c r="P58" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
+    </row>
+    <row r="59" spans="2:15">
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
       <c r="F59" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G59" s="1">
-        <v>29</v>
-      </c>
-      <c r="H59" s="3">
-        <v>54</v>
+        <v>223</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J59" s="1"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="J59" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="K59" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1" t="s">
-        <v>219</v>
+      <c r="N59" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:P59" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P59">
-      <sortCondition sortBy="cellColor" ref="H2:H59" dxfId="1"/>
+  <autoFilter ref="B2:O59" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:O59">
+      <sortCondition ref="H2:H59"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E59">
@@ -3889,30 +3798,30 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="GPIO8">
+    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="GPIO8">
       <formula>NOT(ISERROR(SEARCH("GPIO8",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="14" operator="containsText" text="GPIO7">
+    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="GPIO7">
       <formula>NOT(ISERROR(SEARCH("GPIO7",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="GPIO9">
+    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="GPIO9">
       <formula>NOT(ISERROR(SEARCH("GPIO9",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="GPIO6">
+    <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="GPIO6">
       <formula>NOT(ISERROR(SEARCH("GPIO6",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B44">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="GPIO8">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="GPIO8">
       <formula>NOT(ISERROR(SEARCH("GPIO8",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="GPIO7">
+    <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="GPIO7">
       <formula>NOT(ISERROR(SEARCH("GPIO7",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="GPIO9">
+    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="GPIO9">
       <formula>NOT(ISERROR(SEARCH("GPIO9",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="GPIO6">
+    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="GPIO6">
       <formula>NOT(ISERROR(SEARCH("GPIO6",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3944,7 +3853,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="5:12">
@@ -3952,10 +3861,10 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>248</v>
-      </c>
-      <c r="K11" s="32" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="K11" s="30" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="5:12">
@@ -3963,13 +3872,13 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>245</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="L12" s="32" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="5:12">
@@ -3977,207 +3886,207 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>249</v>
-      </c>
-      <c r="K13" s="32"/>
+        <v>244</v>
+      </c>
+      <c r="K13" s="30"/>
     </row>
     <row r="14" spans="5:12">
       <c r="F14" s="15" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="5:12">
       <c r="F15" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="K15" s="32" t="s">
-        <v>255</v>
+        <v>245</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="F17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="32" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="34" t="s">
+      <c r="F29" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="G29" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="H29" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="I29" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="J29" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="E29" s="34" t="s">
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="33">
+        <v>1</v>
+      </c>
+      <c r="B30" s="33">
+        <v>10</v>
+      </c>
+      <c r="C30" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="D30" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="E30" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="G29" s="34" t="s">
+      <c r="F30" s="31"/>
+      <c r="G30" s="33">
+        <v>10</v>
+      </c>
+      <c r="H30" s="33">
+        <v>0</v>
+      </c>
+      <c r="I30" s="31">
+        <v>0.314</v>
+      </c>
+      <c r="J30" s="34">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="33">
+        <v>2</v>
+      </c>
+      <c r="B31" s="33">
+        <v>10</v>
+      </c>
+      <c r="C31" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="H29" s="34" t="s">
+      <c r="D31" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="E31" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="J29" s="34" t="s">
+      <c r="F31" s="31"/>
+      <c r="G31" s="33">
+        <v>10</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+      <c r="I31" s="31">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="J31" s="34">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="33">
+        <v>3</v>
+      </c>
+      <c r="B32" s="33">
+        <v>10</v>
+      </c>
+      <c r="C32" s="31" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="35">
-        <v>1</v>
-      </c>
-      <c r="B30" s="35">
+      <c r="D32" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="F32" s="31"/>
+      <c r="G32" s="33">
         <v>10</v>
       </c>
-      <c r="C30" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="D30" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="E30" s="33" t="s">
-        <v>267</v>
-      </c>
-      <c r="F30" s="33"/>
-      <c r="G30" s="35">
-        <v>10</v>
-      </c>
-      <c r="H30" s="35">
+      <c r="H32" s="33">
         <v>0</v>
       </c>
-      <c r="I30" s="33">
-        <v>0.314</v>
-      </c>
-      <c r="J30" s="36">
-        <v>3.14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="35">
+      <c r="I32" s="31">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="J32" s="34">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="33">
+        <v>4</v>
+      </c>
+      <c r="B33" s="33">
+        <v>3</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F33" s="31"/>
+      <c r="G33" s="33">
+        <v>3</v>
+      </c>
+      <c r="H33" s="33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="31">
+        <v>0.79</v>
+      </c>
+      <c r="J33" s="34">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="33">
+        <v>5</v>
+      </c>
+      <c r="B34" s="33">
         <v>2</v>
       </c>
-      <c r="B31" s="35">
-        <v>10</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>269</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="35">
-        <v>10</v>
-      </c>
-      <c r="H31" s="35">
+      <c r="C34" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="F34" s="31"/>
+      <c r="G34" s="33">
+        <v>2</v>
+      </c>
+      <c r="H34" s="33">
         <v>0</v>
       </c>
-      <c r="I31" s="33">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="J31" s="36">
-        <v>2.91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="35">
-        <v>3</v>
-      </c>
-      <c r="B32" s="35">
-        <v>10</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="D32" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="35">
-        <v>10</v>
-      </c>
-      <c r="H32" s="35">
-        <v>0</v>
-      </c>
-      <c r="I32" s="33">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="J32" s="36">
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="35">
-        <v>4</v>
-      </c>
-      <c r="B33" s="35">
-        <v>3</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="35">
-        <v>3</v>
-      </c>
-      <c r="H33" s="35">
-        <v>0</v>
-      </c>
-      <c r="I33" s="33">
-        <v>0.79</v>
-      </c>
-      <c r="J33" s="36">
-        <v>2.37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="35">
-        <v>5</v>
-      </c>
-      <c r="B34" s="35">
-        <v>2</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="D34" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="F34" s="33"/>
-      <c r="G34" s="35">
-        <v>2</v>
-      </c>
-      <c r="H34" s="35">
-        <v>0</v>
-      </c>
-      <c r="I34" s="33">
+      <c r="I34" s="31">
         <v>1.5</v>
       </c>
-      <c r="J34" s="36">
+      <c r="J34" s="34">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Menu Paging, Exit to basic/reset
</commit_message>
<xml_diff>
--- a/PCB/TeensyROM pin-reg map.xlsx
+++ b/PCB/TeensyROM pin-reg map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21EE2B4-9576-4F36-83C3-9196B397BAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE79828-8D7C-400E-9DC7-EF639E71EB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Map" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="282">
   <si>
     <t>Teensy 4.0</t>
   </si>
@@ -891,9 +891,6 @@
     <t>Reset out</t>
   </si>
   <si>
-    <t>Change to/from Bi-Dir buffer FET???</t>
-  </si>
-  <si>
     <t>From button</t>
   </si>
   <si>
@@ -918,6 +915,18 @@
       </rPr>
       <t xml:space="preserve"> OC buffer</t>
     </r>
+  </si>
+  <si>
+    <t>Change to Bi-Dir buffer FET???</t>
+  </si>
+  <si>
+    <t>DMA*</t>
+  </si>
+  <si>
+    <t>NMI*</t>
+  </si>
+  <si>
+    <t>IRQ*</t>
   </si>
 </sst>
 </file>
@@ -1174,14 +1183,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{90DC91C5-8A25-4FD1-9045-E2CBF1985420}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1253,14 +1262,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1676,15 +1677,17 @@
   <dimension ref="B1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="1.6640625" customWidth="1"/>
     <col min="2" max="5" width="11.109375" hidden="1" customWidth="1"/>
-    <col min="6" max="10" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="10" width="11.109375" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" style="20" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -1762,26 +1765,26 @@
         <v>36</v>
       </c>
       <c r="C3" s="35">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D3" s="35">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="1">
-        <v>3</v>
+      <c r="G3" s="2">
+        <v>16</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
+      <c r="J3" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="K3" s="19"/>
       <c r="L3" s="1" t="s">
@@ -1800,26 +1803,26 @@
         <v>36</v>
       </c>
       <c r="C4" s="35">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D4" s="35">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="1">
-        <v>2</v>
+      <c r="G4" s="2">
+        <v>17</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>31</v>
+      <c r="J4" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="1" t="s">
@@ -1831,35 +1834,33 @@
       <c r="N4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="21" t="s">
-        <v>237</v>
-      </c>
+      <c r="O4" s="21"/>
     </row>
     <row r="5" spans="2:15">
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="1">
-        <v>4</v>
+        <v>36</v>
+      </c>
+      <c r="G5" s="2">
+        <v>18</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>48</v>
+      <c r="J5" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="K5" s="19"/>
       <c r="L5" s="1" t="s">
@@ -1875,29 +1876,29 @@
     </row>
     <row r="6" spans="2:15">
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="G6" s="2">
+        <v>19</v>
       </c>
       <c r="H6" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>47</v>
+      <c r="J6" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="1" t="s">
@@ -1907,35 +1908,29 @@
         <v>51</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>196</v>
+        <v>55</v>
       </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="1">
-        <v>6</v>
+        <v>36</v>
+      </c>
+      <c r="G7" s="2">
+        <v>20</v>
       </c>
       <c r="H7" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>46</v>
+      <c r="J7" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="K7" s="19"/>
       <c r="L7" s="1" t="s">
@@ -1945,35 +1940,29 @@
         <v>51</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>204</v>
+        <v>55</v>
       </c>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="1">
-        <v>8</v>
+        <v>36</v>
+      </c>
+      <c r="G8" s="2">
+        <v>21</v>
       </c>
       <c r="H8" s="1">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>45</v>
+      <c r="J8" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="K8" s="19"/>
       <c r="L8" s="1" t="s">
@@ -1983,84 +1972,80 @@
         <v>51</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>199</v>
+        <v>55</v>
       </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="2:15">
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="1">
-        <v>10</v>
-      </c>
-      <c r="H9" s="37">
-        <v>6</v>
+        <v>36</v>
+      </c>
+      <c r="G9" s="2">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1">
+        <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>125</v>
-      </c>
+      <c r="J9" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="K9" s="19"/>
       <c r="L9" s="1" t="s">
-        <v>238</v>
+        <v>40</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="O9" s="38" t="s">
-        <v>276</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="O9" s="1"/>
     </row>
     <row r="10" spans="2:15">
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="9">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="G10" s="2">
+        <v>23</v>
       </c>
       <c r="H10" s="1">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>12</v>
+      <c r="J10" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>55</v>
@@ -2069,261 +2054,263 @@
     </row>
     <row r="11" spans="2:15">
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="9">
-        <v>16</v>
+        <v>36</v>
+      </c>
+      <c r="G11" s="2">
+        <v>24</v>
       </c>
       <c r="H11" s="1">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>11</v>
+      <c r="J11" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="K11" s="19"/>
       <c r="L11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>55</v>
+        <v>190</v>
       </c>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="1">
-        <v>11</v>
-      </c>
-      <c r="H12" s="37">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="G12" s="2">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1">
+        <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="19">
-        <v>9</v>
-      </c>
+      <c r="J12" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="K12" s="19"/>
       <c r="L12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G13" s="2">
+        <v>26</v>
       </c>
       <c r="H13" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="9" t="s">
-        <v>7</v>
+      <c r="J13" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="K13" s="19"/>
       <c r="L13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="9">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="G14" s="2">
+        <v>27</v>
       </c>
       <c r="H14" s="1">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J14" s="9" t="s">
-        <v>9</v>
+      <c r="J14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="K14" s="19"/>
       <c r="L14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>12</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D15" s="3">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="9">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="G15" s="2">
+        <v>28</v>
       </c>
       <c r="H15" s="1">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>8</v>
+      <c r="J15" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>55</v>
+        <v>193</v>
       </c>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="9">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="G16" s="2">
+        <v>29</v>
       </c>
       <c r="H16" s="1">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="9" t="s">
-        <v>10</v>
+      <c r="J16" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="K16" s="19"/>
       <c r="L16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="O16" s="1"/>
     </row>
     <row r="17" spans="2:15">
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="1">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D17" s="3">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G17" s="2">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H17" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="K17" s="19"/>
       <c r="L17" s="1" t="s">
@@ -2333,7 +2320,7 @@
         <v>51</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>55</v>
+        <v>198</v>
       </c>
       <c r="O17" s="1"/>
     </row>
@@ -2342,26 +2329,28 @@
         <v>36</v>
       </c>
       <c r="C18" s="1">
-        <v>19</v>
-      </c>
-      <c r="D18" s="1">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D18" s="3">
+        <v>27</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G18" s="2">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H18" s="1">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>210</v>
+        <v>136</v>
       </c>
       <c r="K18" s="19"/>
       <c r="L18" s="1" t="s">
@@ -2371,7 +2360,7 @@
         <v>51</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="O18" s="1"/>
     </row>
@@ -2380,102 +2369,114 @@
         <v>36</v>
       </c>
       <c r="C19" s="1">
-        <v>23</v>
-      </c>
-      <c r="D19" s="1">
-        <v>16</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="D19" s="3">
+        <v>24</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="2">
-        <v>23</v>
+      <c r="G19" s="1">
+        <v>12</v>
       </c>
       <c r="H19" s="1">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="K19" s="19"/>
+      <c r="J19" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K19" s="19">
+        <v>4</v>
+      </c>
       <c r="L19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>51</v>
+        <v>235</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>277</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O19" s="1"/>
+        <v>226</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="20" spans="2:15">
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="1">
-        <v>22</v>
-      </c>
-      <c r="D20" s="1">
-        <v>17</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D20" s="3">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="2">
-        <v>22</v>
-      </c>
-      <c r="H20" s="1">
-        <v>17</v>
+      <c r="G20" s="1">
+        <v>13</v>
+      </c>
+      <c r="H20" s="37">
+        <v>25</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="K20" s="19"/>
+      <c r="J20" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="L20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>51</v>
+        <v>238</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O20" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="1">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="2">
-        <v>17</v>
+      <c r="G21" s="1">
+        <v>2</v>
       </c>
       <c r="H21" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>208</v>
+      <c r="J21" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="K21" s="19"/>
       <c r="L21" s="1" t="s">
@@ -2487,33 +2488,35 @@
       <c r="N21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O21" s="1"/>
+      <c r="O21" s="1" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="22" spans="2:15">
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="2">
-        <v>16</v>
+      <c r="G22" s="1">
+        <v>3</v>
       </c>
       <c r="H22" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>207</v>
+      <c r="J22" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="K22" s="19"/>
       <c r="L22" s="1" t="s">
@@ -2529,321 +2532,311 @@
     </row>
     <row r="23" spans="2:15">
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="2">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>25</v>
+      <c r="J23" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="K23" s="19"/>
       <c r="L23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>191</v>
+        <v>55</v>
       </c>
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="2:15">
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="1">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="2">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="G24" s="9">
+        <v>1</v>
       </c>
       <c r="H24" s="1">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>26</v>
+      <c r="J24" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="K24" s="19"/>
       <c r="L24" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="2:15">
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="2">
-        <v>24</v>
+        <v>37</v>
+      </c>
+      <c r="G25" s="9">
+        <v>2</v>
       </c>
       <c r="H25" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>215</v>
+      <c r="J25" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="K25" s="19"/>
       <c r="L25" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>190</v>
+        <v>55</v>
       </c>
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="2:15">
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="2">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="G26" s="9">
+        <v>3</v>
       </c>
       <c r="H26" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>216</v>
+      <c r="J26" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="K26" s="19"/>
       <c r="L26" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O26" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="27" spans="2:15">
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1">
-        <v>12</v>
-      </c>
-      <c r="D27" s="3">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="1">
-        <v>12</v>
+        <v>37</v>
+      </c>
+      <c r="G27" s="9">
+        <v>16</v>
       </c>
       <c r="H27" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K27" s="19">
-        <v>4</v>
-      </c>
+      <c r="J27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="19"/>
       <c r="L27" s="1" t="s">
-        <v>235</v>
+        <v>41</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>278</v>
+        <v>52</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>234</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="O27" s="1"/>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1">
-        <v>13</v>
-      </c>
-      <c r="D28" s="3">
-        <v>25</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="1">
-        <v>13</v>
-      </c>
-      <c r="H28" s="37">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="G28" s="9">
+        <v>17</v>
+      </c>
+      <c r="H28" s="1">
+        <v>7</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K28" s="19" t="s">
-        <v>127</v>
-      </c>
+      <c r="J28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="19"/>
       <c r="L28" s="1" t="s">
-        <v>238</v>
+        <v>41</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="O28" s="17" t="s">
-        <v>233</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="O28" s="1"/>
     </row>
     <row r="29" spans="2:15">
       <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1">
+        <v>13</v>
+      </c>
+      <c r="D29" s="3">
         <v>36</v>
-      </c>
-      <c r="C29" s="1">
-        <v>30</v>
-      </c>
-      <c r="D29" s="3">
-        <v>26</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="9">
+        <v>18</v>
+      </c>
+      <c r="H29" s="1">
         <v>36</v>
-      </c>
-      <c r="G29" s="2">
-        <v>30</v>
-      </c>
-      <c r="H29" s="1">
-        <v>26</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>140</v>
+      <c r="J29" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="K29" s="19"/>
       <c r="L29" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>198</v>
+        <v>55</v>
       </c>
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="2:15">
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D30" s="3">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="2">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="G30" s="9">
+        <v>19</v>
       </c>
       <c r="H30" s="1">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>136</v>
+      <c r="J30" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="K30" s="19"/>
       <c r="L30" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>195</v>
+        <v>55</v>
       </c>
       <c r="O30" s="1"/>
     </row>
@@ -2852,172 +2845,174 @@
         <v>38</v>
       </c>
       <c r="C31" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D31" s="3">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G31" s="1">
-        <v>18</v>
-      </c>
-      <c r="H31" s="37">
         <v>28</v>
+      </c>
+      <c r="H31" s="1">
+        <v>35</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K31" s="19">
-        <v>6</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="K31" s="19"/>
       <c r="L31" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>236</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="O31" s="1"/>
     </row>
     <row r="32" spans="2:15">
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1">
-        <v>31</v>
-      </c>
-      <c r="D32" s="3">
-        <v>29</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D32" s="1">
+        <v>9</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G32" s="1">
-        <v>31</v>
-      </c>
-      <c r="H32" s="1">
-        <v>29</v>
+        <v>11</v>
+      </c>
+      <c r="H32" s="37">
+        <v>9</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K32" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="K32" s="19">
+        <v>9</v>
+      </c>
       <c r="L32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="O32" s="1"/>
     </row>
     <row r="33" spans="2:15">
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G33" s="1">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H33" s="37">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="K33" s="19">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="M33" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="O33" s="1"/>
     </row>
     <row r="34" spans="2:15">
       <c r="B34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1">
-        <v>22</v>
-      </c>
-      <c r="D34" s="3">
-        <v>31</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6</v>
+      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G34" s="1">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H34" s="37">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J34" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="K34" s="19"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1" t="s">
-        <v>277</v>
+      <c r="J34" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="K34" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O34" s="38" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="35" spans="2:15">
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D35" s="3">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>28</v>
@@ -3026,63 +3021,65 @@
         <v>37</v>
       </c>
       <c r="G35" s="1">
-        <v>12</v>
-      </c>
-      <c r="H35" s="37">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="H35" s="1">
+        <v>34</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K35" s="19">
-        <v>8</v>
-      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="19"/>
       <c r="L35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="M35" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
     <row r="36" spans="2:15">
       <c r="B36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D36" s="3">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G36" s="1">
-        <v>7</v>
-      </c>
-      <c r="H36" s="1">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="H36" s="37">
+        <v>30</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="1"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="N36" s="1"/>
+      <c r="J36" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="K36" s="19">
+        <v>13</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="O36" s="1"/>
     </row>
     <row r="37" spans="2:15">
@@ -3090,234 +3087,186 @@
         <v>38</v>
       </c>
       <c r="C37" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D37" s="3">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G37" s="1">
-        <v>29</v>
-      </c>
-      <c r="H37" s="1">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="H37" s="37">
+        <v>28</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
+      <c r="J37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K37" s="19">
+        <v>6</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="38" spans="2:15">
       <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C38" s="1">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D38" s="3">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G38" s="1">
-        <v>28</v>
-      </c>
-      <c r="H38" s="1">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="H38" s="37">
+        <v>31</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>49</v>
+      <c r="J38" s="16" t="s">
+        <v>274</v>
       </c>
       <c r="K38" s="19"/>
       <c r="L38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="1">
+        <v>15</v>
+      </c>
+      <c r="H39" s="17">
         <v>42</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="I39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="1">
+        <v>14</v>
+      </c>
+      <c r="H40" s="17">
+        <v>43</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="1"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" s="1">
+        <v>13</v>
+      </c>
+      <c r="H41" s="17">
         <v>44</v>
       </c>
-      <c r="N38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O38" s="1"/>
-    </row>
-    <row r="39" spans="2:15">
-      <c r="B39" s="1" t="s">
+      <c r="I41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" s="1"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="1">
-        <v>13</v>
-      </c>
-      <c r="D39" s="3">
-        <v>36</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="G42" s="1">
+        <v>12</v>
+      </c>
+      <c r="H42" s="17">
+        <v>45</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39" s="9">
-        <v>18</v>
-      </c>
-      <c r="H39" s="1">
-        <v>36</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" s="19"/>
-      <c r="L39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O39" s="1"/>
-    </row>
-    <row r="40" spans="2:15">
-      <c r="B40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="1">
-        <v>12</v>
-      </c>
-      <c r="D40" s="3">
-        <v>37</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G40" s="9">
-        <v>19</v>
-      </c>
-      <c r="H40" s="1">
-        <v>37</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K40" s="19"/>
-      <c r="L40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="2:15">
-      <c r="B41" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="1">
-        <v>17</v>
-      </c>
-      <c r="D41" s="3">
-        <v>38</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G41" s="2">
-        <v>28</v>
-      </c>
-      <c r="H41" s="1">
-        <v>38</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K41" s="19"/>
-      <c r="L41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O41" s="1"/>
-    </row>
-    <row r="42" spans="2:15">
-      <c r="B42" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="1">
-        <v>16</v>
-      </c>
-      <c r="D42" s="3">
-        <v>39</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" s="2">
-        <v>29</v>
-      </c>
-      <c r="H42" s="1">
-        <v>39</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="J42" s="1"/>
       <c r="K42" s="19"/>
-      <c r="L42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="O42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="43" spans="2:15">
       <c r="B43" s="1"/>
@@ -3325,31 +3274,25 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G43" s="2">
-        <v>20</v>
-      </c>
-      <c r="H43" s="1">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="G43" s="1">
+        <v>17</v>
+      </c>
+      <c r="H43" s="17">
+        <v>46</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>211</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J43" s="1"/>
       <c r="K43" s="19"/>
-      <c r="L43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="44" spans="2:15">
       <c r="B44" s="1"/>
@@ -3357,187 +3300,253 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G44" s="2">
-        <v>21</v>
-      </c>
-      <c r="H44" s="1">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="G44" s="1">
+        <v>16</v>
+      </c>
+      <c r="H44" s="17">
+        <v>47</v>
       </c>
       <c r="I44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="1"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="1">
+        <v>31</v>
+      </c>
+      <c r="D45" s="3">
+        <v>29</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G45" s="1">
+        <v>31</v>
+      </c>
+      <c r="H45" s="1">
+        <v>29</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="K44" s="19"/>
-      <c r="L44" s="1" t="s">
+      <c r="J45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K45" s="19"/>
+      <c r="L45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O44" s="1"/>
-    </row>
-    <row r="45" spans="2:15">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="1">
-        <v>15</v>
-      </c>
-      <c r="H45" s="17">
-        <v>42</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J45" s="1"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="N45" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O45" s="1"/>
     </row>
     <row r="46" spans="2:15">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2</v>
+      </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G46" s="1">
-        <v>14</v>
-      </c>
-      <c r="H46" s="17">
+        <v>4</v>
+      </c>
+      <c r="H46" s="1">
+        <v>2</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J46" s="1"/>
+      <c r="J46" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="K46" s="19"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="L46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O46" s="1"/>
     </row>
     <row r="47" spans="2:15">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="1">
+        <v>5</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3</v>
+      </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G47" s="1">
-        <v>13</v>
-      </c>
-      <c r="H47" s="17">
-        <v>44</v>
+        <v>5</v>
+      </c>
+      <c r="H47" s="1">
+        <v>3</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J47" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="K47" s="19"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="L47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O47" s="1"/>
     </row>
     <row r="48" spans="2:15">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="1">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>5</v>
+      </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G48" s="1">
-        <v>12</v>
-      </c>
-      <c r="H48" s="17">
+        <v>8</v>
+      </c>
+      <c r="H48" s="1">
+        <v>5</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J48" s="1"/>
       <c r="K48" s="19"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="L48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O48" s="1"/>
     </row>
     <row r="49" spans="2:15">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="1">
+        <v>6</v>
+      </c>
+      <c r="D49" s="1">
+        <v>4</v>
+      </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G49" s="1">
-        <v>17</v>
-      </c>
-      <c r="H49" s="17">
+        <v>6</v>
+      </c>
+      <c r="H49" s="1">
+        <v>4</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="K49" s="19"/>
+      <c r="L49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O49" s="1"/>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="1">
+        <v>7</v>
+      </c>
+      <c r="D50" s="3">
+        <v>33</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G50" s="1">
-        <v>16</v>
-      </c>
-      <c r="H50" s="17">
-        <v>47</v>
+        <v>7</v>
+      </c>
+      <c r="H50" s="1">
+        <v>33</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="19"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
+      <c r="L50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M50" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="N50" s="1"/>
-      <c r="O50" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="O50" s="1"/>
     </row>
     <row r="51" spans="2:15">
       <c r="B51" s="1"/>
@@ -3733,25 +3742,27 @@
         <v>223</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>61</v>
+        <v>222</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K58" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>61</v>
+        <v>221</v>
       </c>
       <c r="M58" s="1"/>
       <c r="N58" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="O58" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="59" spans="2:15">
       <c r="B59" s="36"/>
@@ -3765,32 +3776,30 @@
         <v>223</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>222</v>
+        <v>61</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J59" s="22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K59" s="19" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>221</v>
+        <v>61</v>
       </c>
       <c r="M59" s="1"/>
       <c r="N59" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>220</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="O59" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:O59" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:O59">
-      <sortCondition ref="H2:H59"/>
+      <sortCondition ref="F2:F59"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E59">

</xml_diff>

<commit_message>
Full file transfer via usb for .prg and .crt files (incl parsing/executing)
</commit_message>
<xml_diff>
--- a/PCB/TeensyROM pin-reg map.xlsx
+++ b/PCB/TeensyROM pin-reg map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28416E59-55C6-4BB7-96AD-BE5C689CC95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131C6F65-25A2-4FC1-A3B4-53881E73D869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="-15135" windowWidth="20265" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Map" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="279">
   <si>
     <t>Teensy 4.0</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>T4 LED, OK?</t>
-  </si>
-  <si>
     <t>Direction (From C64)</t>
   </si>
   <si>
@@ -879,6 +876,9 @@
   </si>
   <si>
     <t>LED</t>
+  </si>
+  <si>
+    <t>Teensy LED</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1066,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1128,7 +1128,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1623,7 +1622,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
+      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1636,7 +1635,7 @@
     <col min="11" max="11" width="8.33203125" style="20" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="49.44140625" customWidth="1"/>
+    <col min="15" max="15" width="26.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.3">
@@ -1690,10 +1689,10 @@
         <v>30</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M2" s="28" t="s">
         <v>53</v>
@@ -1715,7 +1714,9 @@
       <c r="D3" s="35">
         <v>19</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>43</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K3" s="19"/>
       <c r="L3" s="1" t="s">
@@ -1753,7 +1754,9 @@
       <c r="D4" s="35">
         <v>18</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>43</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="1" t="s">
@@ -1791,7 +1794,9 @@
       <c r="D5" s="1">
         <v>14</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>43</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K5" s="19"/>
       <c r="L5" s="1" t="s">
@@ -1829,7 +1834,9 @@
       <c r="D6" s="1">
         <v>15</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
@@ -1843,7 +1850,7 @@
         <v>43</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="1" t="s">
@@ -1875,7 +1882,7 @@
         <v>43</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K7" s="19"/>
       <c r="L7" s="1" t="s">
@@ -1907,7 +1914,7 @@
         <v>43</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K8" s="19"/>
       <c r="L8" s="1" t="s">
@@ -1931,7 +1938,9 @@
       <c r="D9" s="1">
         <v>17</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1945,7 +1954,7 @@
         <v>43</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="1" t="s">
@@ -1969,7 +1978,9 @@
       <c r="D10" s="1">
         <v>16</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1983,7 +1994,7 @@
         <v>43</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="1" t="s">
@@ -2007,7 +2018,9 @@
       <c r="D11" s="1">
         <v>22</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>36</v>
       </c>
@@ -2021,7 +2034,7 @@
         <v>43</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K11" s="19"/>
       <c r="L11" s="1" t="s">
@@ -2031,7 +2044,7 @@
         <v>51</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O11" s="1"/>
     </row>
@@ -2045,7 +2058,9 @@
       <c r="D12" s="1">
         <v>23</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2059,7 +2074,7 @@
         <v>43</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K12" s="19"/>
       <c r="L12" s="1" t="s">
@@ -2069,7 +2084,7 @@
         <v>51</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O12" s="1"/>
     </row>
@@ -2083,7 +2098,9 @@
       <c r="D13" s="1">
         <v>20</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2107,7 +2124,7 @@
         <v>51</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O13" s="1"/>
     </row>
@@ -2121,7 +2138,9 @@
       <c r="D14" s="1">
         <v>21</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>36</v>
       </c>
@@ -2145,7 +2164,7 @@
         <v>51</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O14" s="1"/>
     </row>
@@ -2185,7 +2204,7 @@
         <v>51</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O15" s="1"/>
     </row>
@@ -2215,7 +2234,7 @@
         <v>43</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K16" s="19"/>
       <c r="L16" s="1" t="s">
@@ -2225,7 +2244,7 @@
         <v>51</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -2255,7 +2274,7 @@
         <v>43</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K17" s="19"/>
       <c r="L17" s="1" t="s">
@@ -2265,7 +2284,7 @@
         <v>51</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O17" s="1"/>
     </row>
@@ -2295,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K18" s="19"/>
       <c r="L18" s="1" t="s">
@@ -2305,7 +2324,7 @@
         <v>51</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O18" s="1"/>
     </row>
@@ -2335,22 +2354,22 @@
         <v>43</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K19" s="19">
         <v>4</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="O19" s="37" t="s">
-        <v>274</v>
+        <v>223</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
@@ -2379,22 +2398,22 @@
         <v>43</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M20" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="O20" s="37" t="s">
-        <v>275</v>
+        <v>226</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -2407,7 +2426,9 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>36</v>
       </c>
@@ -2434,7 +2455,7 @@
         <v>55</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
@@ -2447,7 +2468,9 @@
       <c r="D22" s="1">
         <v>0</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>36</v>
       </c>
@@ -2485,7 +2508,9 @@
       <c r="D23" s="1">
         <v>10</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F23" s="1" t="s">
         <v>37</v>
       </c>
@@ -2523,7 +2548,9 @@
       <c r="D24" s="1">
         <v>12</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F24" s="1" t="s">
         <v>37</v>
       </c>
@@ -2561,7 +2588,9 @@
       <c r="D25" s="1">
         <v>11</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>37</v>
       </c>
@@ -2599,7 +2628,9 @@
       <c r="D26" s="1">
         <v>13</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>37</v>
       </c>
@@ -2626,7 +2657,7 @@
         <v>55</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>57</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
@@ -2639,7 +2670,9 @@
       <c r="D27" s="1">
         <v>8</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>37</v>
       </c>
@@ -2677,7 +2710,9 @@
       <c r="D28" s="1">
         <v>7</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>37</v>
       </c>
@@ -2835,7 +2870,9 @@
       <c r="D32" s="1">
         <v>9</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F32" s="1" t="s">
         <v>37</v>
       </c>
@@ -2861,7 +2898,7 @@
         <v>50</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O32" s="1"/>
     </row>
@@ -2903,7 +2940,7 @@
         <v>50</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O33" s="1"/>
     </row>
@@ -2917,7 +2954,9 @@
       <c r="D34" s="1">
         <v>6</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>37</v>
       </c>
@@ -2931,22 +2970,22 @@
         <v>43</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="O34" s="37" t="s">
-        <v>274</v>
+        <v>199</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
@@ -2975,14 +3014,14 @@
         <v>43</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K35" s="19"/>
-      <c r="L35" s="37" t="s">
+      <c r="L35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M35" s="37" t="s">
-        <v>278</v>
+      <c r="M35" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -3013,19 +3052,19 @@
         <v>43</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K36" s="19">
         <v>13</v>
       </c>
-      <c r="L36" s="37" t="s">
+      <c r="L36" s="1" t="s">
         <v>42</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O36" s="1"/>
     </row>
@@ -3055,22 +3094,22 @@
         <v>43</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K37" s="19">
         <v>6</v>
       </c>
-      <c r="L37" s="37" t="s">
+      <c r="L37" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
@@ -3098,15 +3137,15 @@
       <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="37" t="s">
-        <v>276</v>
+      <c r="J38" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="K38" s="19"/>
-      <c r="L38" s="37" t="s">
+      <c r="L38" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -3130,11 +3169,11 @@
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="19"/>
-      <c r="L39" s="37"/>
+      <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
@@ -3156,11 +3195,11 @@
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="19"/>
-      <c r="L40" s="37"/>
+      <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
@@ -3182,11 +3221,11 @@
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="19"/>
-      <c r="L41" s="37"/>
+      <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.3">
@@ -3208,11 +3247,11 @@
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="19"/>
-      <c r="L42" s="37"/>
+      <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.3">
@@ -3234,11 +3273,11 @@
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="19"/>
-      <c r="L43" s="37"/>
+      <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.3">
@@ -3260,11 +3299,11 @@
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="19"/>
-      <c r="L44" s="37"/>
+      <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.3">
@@ -3293,17 +3332,17 @@
         <v>43</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K45" s="19"/>
-      <c r="L45" s="37" t="s">
+      <c r="L45" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O45" s="1"/>
     </row>
@@ -3317,7 +3356,9 @@
       <c r="D46" s="1">
         <v>2</v>
       </c>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F46" s="1" t="s">
         <v>39</v>
       </c>
@@ -3334,7 +3375,7 @@
         <v>48</v>
       </c>
       <c r="K46" s="19"/>
-      <c r="L46" s="37" t="s">
+      <c r="L46" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M46" s="1" t="s">
@@ -3355,7 +3396,9 @@
       <c r="D47" s="1">
         <v>3</v>
       </c>
-      <c r="E47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F47" s="1" t="s">
         <v>39</v>
       </c>
@@ -3372,14 +3415,14 @@
         <v>47</v>
       </c>
       <c r="K47" s="19"/>
-      <c r="L47" s="37" t="s">
+      <c r="L47" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O47" s="1"/>
     </row>
@@ -3393,7 +3436,9 @@
       <c r="D48" s="1">
         <v>5</v>
       </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F48" s="1" t="s">
         <v>39</v>
       </c>
@@ -3410,14 +3455,14 @@
         <v>45</v>
       </c>
       <c r="K48" s="19"/>
-      <c r="L48" s="37" t="s">
+      <c r="L48" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O48" s="1"/>
     </row>
@@ -3431,7 +3476,9 @@
       <c r="D49" s="1">
         <v>4</v>
       </c>
-      <c r="E49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F49" s="1" t="s">
         <v>39</v>
       </c>
@@ -3448,14 +3495,14 @@
         <v>46</v>
       </c>
       <c r="K49" s="19"/>
-      <c r="L49" s="37" t="s">
+      <c r="L49" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M49" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O49" s="1"/>
     </row>
@@ -3485,14 +3532,14 @@
         <v>43</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K50" s="19"/>
-      <c r="L50" s="37" t="s">
+      <c r="L50" s="1" t="s">
         <v>42</v>
       </c>
       <c r="M50" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
@@ -3520,7 +3567,7 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.3">
@@ -3546,7 +3593,7 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.3">
@@ -3572,7 +3619,7 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.3">
@@ -3598,7 +3645,7 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.3">
@@ -3624,7 +3671,7 @@
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
@@ -3650,7 +3697,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.3">
@@ -3676,7 +3723,7 @@
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
@@ -3685,32 +3732,32 @@
       <c r="D58" s="36"/>
       <c r="E58" s="36"/>
       <c r="F58" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K58" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M58" s="1"/>
       <c r="N58" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.3">
@@ -3719,29 +3766,29 @@
       <c r="D59" s="36"/>
       <c r="E59" s="36"/>
       <c r="F59" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J59" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K59" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M59" s="1"/>
       <c r="N59" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O59" s="1"/>
     </row>
@@ -3811,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="5:12" x14ac:dyDescent="0.3">
@@ -3819,10 +3866,10 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K11" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="5:12" x14ac:dyDescent="0.3">
@@ -3830,13 +3877,13 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
+        <v>234</v>
+      </c>
+      <c r="K12" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="K12" s="30" t="s">
-        <v>236</v>
-      </c>
       <c r="L12" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="5:12" x14ac:dyDescent="0.3">
@@ -3844,58 +3891,58 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K13" s="30"/>
     </row>
     <row r="14" spans="5:12" x14ac:dyDescent="0.3">
       <c r="F14" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="5:12" x14ac:dyDescent="0.3">
       <c r="F15" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K15" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B29" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="C29" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="D29" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="E29" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="F29" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="G29" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="H29" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="I29" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="I29" s="32" t="s">
+      <c r="J29" s="32" t="s">
         <v>253</v>
-      </c>
-      <c r="J29" s="32" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -3906,13 +3953,13 @@
         <v>10</v>
       </c>
       <c r="C30" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="E30" s="31" t="s">
         <v>255</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="E30" s="31" t="s">
-        <v>256</v>
       </c>
       <c r="F30" s="31"/>
       <c r="G30" s="33">
@@ -3936,13 +3983,13 @@
         <v>10</v>
       </c>
       <c r="C31" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="D31" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="E31" s="31" t="s">
         <v>258</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>259</v>
       </c>
       <c r="F31" s="31"/>
       <c r="G31" s="33">
@@ -3966,13 +4013,13 @@
         <v>10</v>
       </c>
       <c r="C32" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="D32" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="E32" s="31" t="s">
         <v>261</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>262</v>
       </c>
       <c r="F32" s="31"/>
       <c r="G32" s="33">
@@ -3996,13 +4043,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="D33" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="E33" s="31" t="s">
         <v>264</v>
-      </c>
-      <c r="E33" s="31" t="s">
-        <v>265</v>
       </c>
       <c r="F33" s="31"/>
       <c r="G33" s="33">
@@ -4026,13 +4073,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D34" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="E34" s="31" t="s">
         <v>267</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>268</v>
       </c>
       <c r="F34" s="31"/>
       <c r="G34" s="33">
@@ -4086,13 +4133,13 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
         <v>58</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>59</v>
-      </c>
-      <c r="F8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -4100,16 +4147,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>63</v>
-      </c>
-      <c r="F9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -4117,16 +4164,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>66</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -4134,16 +4181,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
         <v>65</v>
       </c>
-      <c r="D11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>66</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -4151,16 +4198,16 @@
         <v>4</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
         <v>41</v>
       </c>
       <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
         <v>69</v>
-      </c>
-      <c r="F12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
@@ -4168,16 +4215,16 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
         <v>41</v>
       </c>
       <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
         <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -4185,16 +4232,16 @@
         <v>6</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
         <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -4202,16 +4249,16 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
       </c>
       <c r="E15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" t="s">
         <v>77</v>
-      </c>
-      <c r="F15" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -4219,16 +4266,16 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
         <v>40</v>
       </c>
       <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
         <v>80</v>
-      </c>
-      <c r="F16" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -4236,16 +4283,16 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
         <v>40</v>
       </c>
       <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
         <v>83</v>
-      </c>
-      <c r="F17" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -4253,16 +4300,16 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
       </c>
       <c r="E18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" t="s">
         <v>86</v>
-      </c>
-      <c r="F18" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -4270,16 +4317,16 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
       </c>
       <c r="E19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
         <v>89</v>
-      </c>
-      <c r="F19" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -4287,16 +4334,16 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -4304,16 +4351,16 @@
         <v>13</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
         <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -4321,16 +4368,16 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
         <v>41</v>
       </c>
       <c r="E22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" t="s">
         <v>96</v>
-      </c>
-      <c r="F22" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -4338,16 +4385,16 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
         <v>99</v>
-      </c>
-      <c r="F23" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -4355,16 +4402,16 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
         <v>41</v>
       </c>
       <c r="E24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" t="s">
         <v>102</v>
-      </c>
-      <c r="F24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
@@ -4372,16 +4419,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
         <v>41</v>
       </c>
       <c r="E25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" t="s">
         <v>105</v>
-      </c>
-      <c r="F25" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -4389,16 +4436,16 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
         <v>41</v>
       </c>
       <c r="E26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" t="s">
         <v>108</v>
-      </c>
-      <c r="F26" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
@@ -4406,16 +4453,16 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
         <v>41</v>
       </c>
       <c r="E27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" t="s">
         <v>111</v>
-      </c>
-      <c r="F27" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
@@ -4423,16 +4470,16 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
         <v>41</v>
       </c>
       <c r="E28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" t="s">
         <v>114</v>
-      </c>
-      <c r="F28" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
@@ -4440,16 +4487,16 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
         <v>41</v>
       </c>
       <c r="E29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" t="s">
         <v>117</v>
-      </c>
-      <c r="F29" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
@@ -4457,58 +4504,58 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
         <v>61</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>62</v>
       </c>
-      <c r="E30" t="s">
-        <v>63</v>
-      </c>
       <c r="F30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
         <v>61</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>62</v>
       </c>
-      <c r="E31" t="s">
-        <v>63</v>
-      </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s">
         <v>121</v>
-      </c>
-      <c r="C32" t="s">
-        <v>122</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
       </c>
       <c r="E32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" t="s">
         <v>123</v>
-      </c>
-      <c r="F32" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s">
         <v>125</v>
-      </c>
-      <c r="C33" t="s">
-        <v>126</v>
       </c>
       <c r="D33" t="s">
         <v>40</v>
@@ -4517,97 +4564,97 @@
         <v>33</v>
       </c>
       <c r="F33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="D34" t="s">
         <v>40</v>
       </c>
       <c r="E34" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" t="s">
         <v>129</v>
-      </c>
-      <c r="F34" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" t="s">
         <v>131</v>
-      </c>
-      <c r="C35" t="s">
-        <v>132</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
       </c>
       <c r="E35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" t="s">
         <v>133</v>
-      </c>
-      <c r="F35" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" t="s">
         <v>135</v>
-      </c>
-      <c r="C36" t="s">
-        <v>136</v>
       </c>
       <c r="D36" t="s">
         <v>41</v>
       </c>
       <c r="E36" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" t="s">
         <v>137</v>
-      </c>
-      <c r="F36" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" t="s">
         <v>139</v>
-      </c>
-      <c r="C37" t="s">
-        <v>140</v>
       </c>
       <c r="D37" t="s">
         <v>41</v>
       </c>
       <c r="E37" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" t="s">
         <v>141</v>
-      </c>
-      <c r="F37" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" t="s">
         <v>143</v>
-      </c>
-      <c r="C38" t="s">
-        <v>144</v>
       </c>
       <c r="D38" t="s">
         <v>41</v>
       </c>
       <c r="E38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" t="s">
         <v>145</v>
-      </c>
-      <c r="F38" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
@@ -4616,15 +4663,15 @@
         <v>41</v>
       </c>
       <c r="E39" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" t="s">
         <v>148</v>
-      </c>
-      <c r="F39" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
         <v>26</v>
@@ -4633,15 +4680,15 @@
         <v>41</v>
       </c>
       <c r="E40" t="s">
+        <v>150</v>
+      </c>
+      <c r="F40" t="s">
         <v>151</v>
-      </c>
-      <c r="F40" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
@@ -4650,15 +4697,15 @@
         <v>41</v>
       </c>
       <c r="E41" t="s">
+        <v>153</v>
+      </c>
+      <c r="F41" t="s">
         <v>154</v>
-      </c>
-      <c r="F41" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -4667,15 +4714,15 @@
         <v>41</v>
       </c>
       <c r="E42" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" t="s">
         <v>157</v>
-      </c>
-      <c r="F42" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -4684,15 +4731,15 @@
         <v>41</v>
       </c>
       <c r="E43" t="s">
+        <v>159</v>
+      </c>
+      <c r="F43" t="s">
         <v>160</v>
-      </c>
-      <c r="F43" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C44" t="s">
         <v>22</v>
@@ -4701,15 +4748,15 @@
         <v>41</v>
       </c>
       <c r="E44" t="s">
+        <v>162</v>
+      </c>
+      <c r="F44" t="s">
         <v>163</v>
-      </c>
-      <c r="F44" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C45" t="s">
         <v>21</v>
@@ -4718,15 +4765,15 @@
         <v>41</v>
       </c>
       <c r="E45" t="s">
+        <v>165</v>
+      </c>
+      <c r="F45" t="s">
         <v>166</v>
-      </c>
-      <c r="F45" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C46" t="s">
         <v>20</v>
@@ -4735,15 +4782,15 @@
         <v>41</v>
       </c>
       <c r="E46" t="s">
+        <v>168</v>
+      </c>
+      <c r="F46" t="s">
         <v>169</v>
-      </c>
-      <c r="F46" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
         <v>19</v>
@@ -4752,15 +4799,15 @@
         <v>41</v>
       </c>
       <c r="E47" t="s">
+        <v>171</v>
+      </c>
+      <c r="F47" t="s">
         <v>172</v>
-      </c>
-      <c r="F47" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C48" t="s">
         <v>18</v>
@@ -4769,15 +4816,15 @@
         <v>41</v>
       </c>
       <c r="E48" t="s">
+        <v>174</v>
+      </c>
+      <c r="F48" t="s">
         <v>175</v>
-      </c>
-      <c r="F48" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
@@ -4786,10 +4833,10 @@
         <v>41</v>
       </c>
       <c r="E49" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" t="s">
         <v>178</v>
-      </c>
-      <c r="F49" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
@@ -4803,15 +4850,15 @@
         <v>41</v>
       </c>
       <c r="E50" t="s">
+        <v>179</v>
+      </c>
+      <c r="F50" t="s">
         <v>180</v>
-      </c>
-      <c r="F50" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
@@ -4820,27 +4867,27 @@
         <v>41</v>
       </c>
       <c r="E51" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" t="s">
         <v>183</v>
-      </c>
-      <c r="F51" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C52" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" t="s">
         <v>61</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>62</v>
       </c>
-      <c r="E52" t="s">
-        <v>63</v>
-      </c>
       <c r="F52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>